<commit_message>
fixing data pengiriman excel dengan validasi format no hp
</commit_message>
<xml_diff>
--- a/public/excel_format/DataPengiriman.xlsx
+++ b/public/excel_format/DataPengiriman.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/project-expedisi/public/excel_format/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8E8AA6-6E62-1243-81C0-87CF4E538E3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4B63EE-0F07-BA4A-9B7D-DB0A5B4BBD1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -205,6 +205,7 @@
       <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -212,6 +213,7 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -564,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:T6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -576,7 +578,7 @@
     <col min="6" max="6" width="13.1640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="15.1640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="13.1640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5" style="1" customWidth="1"/>
     <col min="10" max="10" width="15.1640625" style="1" customWidth="1"/>
     <col min="11" max="13" width="13.1640625" style="1" customWidth="1"/>
     <col min="14" max="14" width="18.5" style="1" customWidth="1"/>
@@ -672,10 +674,10 @@
         <v>22</v>
       </c>
       <c r="I2" s="2">
-        <v>81627364536</v>
+        <v>6281627364523</v>
       </c>
       <c r="J2" s="2">
-        <v>81726354728</v>
+        <v>6281726354728</v>
       </c>
       <c r="K2" s="2">
         <v>2.2999999999999998</v>
@@ -729,10 +731,10 @@
         <v>33</v>
       </c>
       <c r="I3" s="2">
-        <v>87564637261</v>
+        <v>6287564637261</v>
       </c>
       <c r="J3" s="2">
-        <v>81274657487</v>
+        <v>6281274657487</v>
       </c>
       <c r="K3" s="2">
         <v>1</v>
@@ -786,10 +788,10 @@
         <v>39</v>
       </c>
       <c r="I4" s="2">
-        <v>81254647587</v>
+        <v>6281254647587</v>
       </c>
       <c r="J4" s="2">
-        <v>87364758676</v>
+        <v>6287364758676</v>
       </c>
       <c r="K4" s="2">
         <v>1</v>
@@ -843,10 +845,10 @@
         <v>44</v>
       </c>
       <c r="I5" s="2">
-        <v>8717267643</v>
+        <v>628717267643</v>
       </c>
       <c r="J5" s="2">
-        <v>82736457485</v>
+        <v>6282736457485</v>
       </c>
       <c r="K5" s="2">
         <v>1.5</v>
@@ -900,10 +902,10 @@
         <v>49</v>
       </c>
       <c r="I6" s="2">
-        <v>81672537485</v>
+        <v>6281672537485</v>
       </c>
       <c r="J6" s="2">
-        <v>8172645362</v>
+        <v>628172645362</v>
       </c>
       <c r="K6" s="2">
         <v>3</v>

</xml_diff>

<commit_message>
update format excel & konfirmasi excel
</commit_message>
<xml_diff>
--- a/public/excel_format/DataPengiriman.xlsx
+++ b/public/excel_format/DataPengiriman.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/project-expedisi/public/excel_format/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4B63EE-0F07-BA4A-9B7D-DB0A5B4BBD1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03842A5D-96F3-8E4C-B385-92EC0BFF6581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,9 +76,6 @@
     <t>keterangan</t>
   </si>
   <si>
-    <t>JHD1827183614</t>
-  </si>
-  <si>
     <t>LP-001</t>
   </si>
   <si>
@@ -94,9 +91,6 @@
     <t>Transfer</t>
   </si>
   <si>
-    <t>BRI</t>
-  </si>
-  <si>
     <t>https://drive.google.com/file/d/1rlz8NoT_I5z39jfG_7XmV_AODeJWbgsL/view?usp=sharing</t>
   </si>
   <si>
@@ -109,9 +103,6 @@
     <t>BKD</t>
   </si>
   <si>
-    <t>JHD9183917419</t>
-  </si>
-  <si>
     <t>General</t>
   </si>
   <si>
@@ -127,9 +118,6 @@
     <t>https://drive.google.com/file/d/1cTYrHijN5tEx-Ls5GWJJ63faUtoWuGAK/view?usp=sharing</t>
   </si>
   <si>
-    <t>JHD9138927422</t>
-  </si>
-  <si>
     <t>LP-002</t>
   </si>
   <si>
@@ -145,9 +133,6 @@
     <t>YA</t>
   </si>
   <si>
-    <t>JHD7927492748</t>
-  </si>
-  <si>
     <t>Jo</t>
   </si>
   <si>
@@ -160,9 +145,6 @@
     <t>BOSSPACK</t>
   </si>
   <si>
-    <t>JHD1827818614</t>
-  </si>
-  <si>
     <t>Heru</t>
   </si>
   <si>
@@ -179,18 +161,43 @@
   </si>
   <si>
     <t>Kasir 2</t>
+  </si>
+  <si>
+    <t>BCA</t>
+  </si>
+  <si>
+    <t>JHD1827183654</t>
+  </si>
+  <si>
+    <t>JHD1827183655</t>
+  </si>
+  <si>
+    <t>JHD1827183656</t>
+  </si>
+  <si>
+    <t>JHD1827183657</t>
+  </si>
+  <si>
+    <t>JHD1827183658</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -264,11 +271,11 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -279,13 +286,22 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -566,27 +582,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:T6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" style="1" customWidth="1"/>
-    <col min="3" max="5" width="15.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.1640625" style="1" customWidth="1"/>
-    <col min="11" max="13" width="13.1640625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="18.5" style="1" customWidth="1"/>
+    <col min="3" max="4" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" style="1" customWidth="1"/>
+    <col min="7" max="8" width="15.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" style="1" customWidth="1"/>
+    <col min="11" max="12" width="13.1640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="18.5" style="1" customWidth="1"/>
+    <col min="14" max="14" width="75.33203125" style="1" customWidth="1"/>
     <col min="15" max="15" width="13.1640625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="75.33203125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="15.5" style="1" customWidth="1"/>
-    <col min="18" max="18" width="13.1640625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="16.1640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="13.1640625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="16.1640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.1640625" style="1" customWidth="1"/>
     <col min="20" max="20" width="20.83203125" style="1" customWidth="1"/>
     <col min="21" max="21" width="13.1640625" style="1" customWidth="1"/>
     <col min="22" max="16384" width="13.1640625" style="1"/>
@@ -599,26 +616,26 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="F1" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="J1" s="2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>8</v>
@@ -627,57 +644,57 @@
         <v>9</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>13</v>
+      <c r="P1" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="T1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="2:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="9">
+        <v>45532.382118055553</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="3">
-        <v>45410</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="2">
+        <v>6281627364523</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2">
+        <v>6281726354728</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="2">
-        <v>6281627364523</v>
-      </c>
-      <c r="J2" s="2">
-        <v>6281726354728</v>
+      <c r="J2" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="K2" s="2">
         <v>2.2999999999999998</v>
@@ -685,56 +702,56 @@
       <c r="L2" s="2">
         <v>26000</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S2" s="2">
         <v>6000</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="T2" s="2"/>
     </row>
     <row r="3" spans="2:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="9">
+        <v>45533.382117997688</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="2">
+        <v>6287564637261</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="3">
-        <v>45411</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="H3" s="2">
+        <v>6281274657487</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" s="2">
-        <v>6287564637261</v>
-      </c>
-      <c r="J3" s="2">
-        <v>6281274657487</v>
+      <c r="J3" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="K3" s="2">
         <v>1</v>
@@ -742,56 +759,56 @@
       <c r="L3" s="2">
         <v>17000</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S3" s="2">
         <v>6000</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="T3" s="2"/>
     </row>
     <row r="4" spans="2:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="9">
+        <v>45534.382117997688</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="2">
+        <v>6281254647587</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="2">
+        <v>6287364758676</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="3">
-        <v>45412</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I4" s="2">
-        <v>6281254647587</v>
-      </c>
-      <c r="J4" s="2">
-        <v>6287364758676</v>
+      <c r="J4" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="K4" s="2">
         <v>1</v>
@@ -799,56 +816,56 @@
       <c r="L4" s="2">
         <v>40000</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S4" s="2">
         <v>4000</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="T4" s="2"/>
     </row>
     <row r="5" spans="2:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="B5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="3">
-        <v>45413</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="B5" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>42</v>
+      <c r="C5" s="9">
+        <v>45535.382117997688</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="2">
+        <v>628717267643</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5" s="2">
-        <v>628717267643</v>
-      </c>
-      <c r="J5" s="2">
+        <v>38</v>
+      </c>
+      <c r="H5" s="2">
         <v>6282736457485</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="K5" s="2">
         <v>1.5</v>
@@ -856,56 +873,56 @@
       <c r="L5" s="2">
         <v>20000</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S5" s="2">
         <v>7000</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="T5" s="2"/>
     </row>
     <row r="6" spans="2:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="B6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" s="3">
-        <v>45409</v>
-      </c>
-      <c r="D6" s="6" t="s">
+      <c r="B6" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>47</v>
+      <c r="C6" s="9">
+        <v>45536.382117997688</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="2">
+        <v>6281672537485</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I6" s="2">
-        <v>6281672537485</v>
-      </c>
-      <c r="J6" s="2">
+        <v>42</v>
+      </c>
+      <c r="H6" s="2">
         <v>628172645362</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="K6" s="2">
         <v>3</v>
@@ -913,35 +930,35 @@
       <c r="L6" s="2">
         <v>35000</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S6" s="2">
         <v>5000</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="T6" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="P4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="P6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="N2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="N4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="N6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update excel format data pengiriman
</commit_message>
<xml_diff>
--- a/public/excel_format/DataPengiriman.xlsx
+++ b/public/excel_format/DataPengiriman.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/project-expedisi/public/excel_format/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03842A5D-96F3-8E4C-B385-92EC0BFF6581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC13EFC8-868B-984E-9C1B-413770868658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="56">
   <si>
     <t>no_resi</t>
   </si>
@@ -166,31 +166,47 @@
     <t>BCA</t>
   </si>
   <si>
-    <t>JHD1827183654</t>
-  </si>
-  <si>
-    <t>JHD1827183655</t>
-  </si>
-  <si>
-    <t>JHD1827183656</t>
-  </si>
-  <si>
-    <t>JHD1827183657</t>
-  </si>
-  <si>
-    <t>JHD1827183658</t>
+    <t>status_kirim_wa</t>
+  </si>
+  <si>
+    <t>Ya</t>
+  </si>
+  <si>
+    <t>Tidak</t>
+  </si>
+  <si>
+    <t>JHD1827183971</t>
+  </si>
+  <si>
+    <t>JHD1827183972</t>
+  </si>
+  <si>
+    <t>JHD1827183973</t>
+  </si>
+  <si>
+    <t>JHD1827183974</t>
+  </si>
+  <si>
+    <t>JHD1827183975</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -271,11 +287,11 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -286,22 +302,25 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -580,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:T6"/>
+  <dimension ref="B1:U6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -603,13 +622,13 @@
     <col min="16" max="16" width="15.6640625" style="1" customWidth="1"/>
     <col min="17" max="17" width="13.1640625" style="1" customWidth="1"/>
     <col min="18" max="18" width="16.1640625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.1640625" style="1" customWidth="1"/>
-    <col min="20" max="20" width="20.83203125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="13.1640625" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="13.1640625" style="1"/>
+    <col min="19" max="20" width="13.1640625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="20.83203125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="13.1640625" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="13.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:21" ht="34" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -664,13 +683,16 @@
       <c r="S1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="2:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="B2" s="8" t="s">
-        <v>48</v>
+    <row r="2" spans="2:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="B2" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="C2" s="9">
         <v>45532.382118055553</v>
@@ -723,11 +745,14 @@
       <c r="S2" s="2">
         <v>6000</v>
       </c>
-      <c r="T2" s="2"/>
+      <c r="T2" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="U2" s="2"/>
     </row>
-    <row r="3" spans="2:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="B3" s="8" t="s">
-        <v>49</v>
+    <row r="3" spans="2:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="B3" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="C3" s="9">
         <v>45533.382117997688</v>
@@ -780,11 +805,14 @@
       <c r="S3" s="2">
         <v>6000</v>
       </c>
-      <c r="T3" s="2"/>
+      <c r="T3" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="U3" s="2"/>
     </row>
-    <row r="4" spans="2:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="B4" s="8" t="s">
-        <v>50</v>
+    <row r="4" spans="2:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="B4" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="C4" s="9">
         <v>45534.382117997688</v>
@@ -837,11 +865,14 @@
       <c r="S4" s="2">
         <v>4000</v>
       </c>
-      <c r="T4" s="2"/>
+      <c r="T4" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="U4" s="2"/>
     </row>
-    <row r="5" spans="2:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="B5" s="8" t="s">
-        <v>51</v>
+    <row r="5" spans="2:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="B5" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="C5" s="9">
         <v>45535.382117997688</v>
@@ -894,11 +925,14 @@
       <c r="S5" s="2">
         <v>7000</v>
       </c>
-      <c r="T5" s="2"/>
+      <c r="T5" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="U5" s="2"/>
     </row>
-    <row r="6" spans="2:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="B6" s="8" t="s">
-        <v>52</v>
+    <row r="6" spans="2:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="B6" s="10" t="s">
+        <v>55</v>
       </c>
       <c r="C6" s="9">
         <v>45536.382117997688</v>
@@ -951,10 +985,13 @@
       <c r="S6" s="2">
         <v>5000</v>
       </c>
-      <c r="T6" s="2"/>
+      <c r="T6" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="U6" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="N2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="N4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>

</xml_diff>